<commit_message>
Promena na nadomest za organizacija
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -736,15 +736,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>360</xdr:colOff>
+      <xdr:colOff>720</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>56880</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>761400</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>175680</xdr:rowOff>
+      <xdr:rowOff>175320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -757,8 +757,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="380520" y="0"/>
-          <a:ext cx="8285040" cy="747000"/>
+          <a:off x="380880" y="0"/>
+          <a:ext cx="8284680" cy="746640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -780,15 +780,16 @@
   </sheetPr>
   <dimension ref="B1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I65" activeCellId="0" sqref="I65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="4.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="4" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.35"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.85"/>
@@ -871,10 +872,12 @@
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="6" t="s">
         <v>1</v>
       </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
@@ -1759,9 +1762,10 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="38">
+  <mergeCells count="41">
     <mergeCell ref="B4:F6"/>
     <mergeCell ref="G4:K6"/>
+    <mergeCell ref="B7:D7"/>
     <mergeCell ref="H7:K7"/>
     <mergeCell ref="B8:F9"/>
     <mergeCell ref="I8:K8"/>
@@ -1795,9 +1799,11 @@
     <mergeCell ref="F55:H55"/>
     <mergeCell ref="I55:K57"/>
     <mergeCell ref="B56:E56"/>
+    <mergeCell ref="F56:H56"/>
     <mergeCell ref="B57:E57"/>
     <mergeCell ref="F57:H57"/>
     <mergeCell ref="B58:E58"/>
+    <mergeCell ref="F58:H58"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>